<commit_message>
xong phan giam sat
</commit_message>
<xml_diff>
--- a/info/logData/Record adila.xlsx
+++ b/info/logData/Record adila.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCompany\8.SourceCode\3.Projects\20220820aldilaTipOdFreqMrDiepMrKhai\info\logData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC603E8-35BF-4926-A3D7-BA536610BA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4245" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto Sanding" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>Shaft Number</t>
   </si>
@@ -247,12 +248,6 @@
     <t>Tất cả các thanh ghi sử dụng data type: Unsigned 16BIN</t>
   </si>
   <si>
-    <t>Bit báo nhận data: d876.0 ( mới thêm vào khi bắt đầu quét barcode đọc data ON bit này lên)</t>
-  </si>
-  <si>
-    <t>Bit reset nhận data: d877.0 (mới thêm vào nhận data xong reset D876.0)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> D872 ( Read Diam OD) để xem giá trị OD hiện tại ko lưu thanh ghi này</t>
   </si>
   <si>
@@ -268,9 +263,6 @@
     <t>Bit báo nhận data: d907.0 ( mới thêm vào khi bắt đầu quét barcode đọc data ON bit này lên)</t>
   </si>
   <si>
-    <t>Bit reset nhận data: d908.0 (mới thêm vào nhận data xong reset D908.0)</t>
-  </si>
-  <si>
     <t>Freq- Target Sand</t>
   </si>
   <si>
@@ -284,18 +276,12 @@
   </si>
   <si>
     <t>Giữ Nguyên</t>
-  </si>
-  <si>
-    <t>Bit báo nhận data: d912.0 ( mới thêm vào khi bắt đầu quét barcode đọc data ON bit này lên)</t>
-  </si>
-  <si>
-    <t>Bit reset nhận data: d913.0 (mới thêm vào nhận data xong reset D912.0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,10 +333,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,11 +616,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +665,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -719,131 +705,120 @@
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="A6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
+      <c r="A13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>49</v>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
       <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -851,11 +826,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,26 +972,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1030,7 +1001,7 @@
     </row>
     <row r="11" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1113,10 +1084,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1155,10 +1126,10 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1195,35 +1166,31 @@
     </row>
     <row r="4" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1259,7 +1226,7 @@
     </row>
     <row r="14" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>